<commit_message>
Added loop for each data to search
</commit_message>
<xml_diff>
--- a/Docs/Details.xlsx
+++ b/Docs/Details.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Prashant\XLNC\MyProjects\LinkedIn\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XLNC\Documents\UiPath\LinkedInBot\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -42,18 +42,12 @@
   </si>
   <si>
     <t>Pr@shant@23101995</t>
-  </si>
-  <si>
-    <t>SearchKeyword</t>
-  </si>
-  <si>
-    <t>data scientist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -365,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -379,7 +373,7 @@
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,11 +383,8 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -402,9 +393,6 @@
       </c>
       <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started with withdraw bot
</commit_message>
<xml_diff>
--- a/Docs/Details.xlsx
+++ b/Docs/Details.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>Pr@shant@23101995</t>
+  </si>
+  <si>
+    <t>Withdraw</t>
+  </si>
+  <si>
+    <t>1 month</t>
   </si>
 </sst>
 </file>
@@ -359,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,7 +379,7 @@
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -383,8 +389,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -393,6 +402,9 @@
       </c>
       <c r="C2" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Processed Data and working on Custom sending connects
</commit_message>
<xml_diff>
--- a/Docs/Details.xlsx
+++ b/Docs/Details.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XLNC\Documents\UiPath\LinkedInBot\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prashant\Documents\UiPath\LinkedInBot\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849152CB-CEB3-41B7-A168-079C1A2A4F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -48,12 +49,18 @@
   </si>
   <si>
     <t>1 month</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -364,11 +371,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -379,7 +386,7 @@
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -392,8 +399,11 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -405,6 +415,9 @@
       </c>
       <c r="D2" t="s">
         <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>